<commit_message>
Cuestionario Part II + PPT PEI
</commit_message>
<xml_diff>
--- a/Cuestionario - Part II.xlsx
+++ b/Cuestionario - Part II.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\CharlaConChris\TestOrientedDevelopment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\TestOrientedDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Designing Testable Applications - Cuestionario</t>
   </si>
@@ -77,9 +77,6 @@
     <t>b) Este método se puede testear unitariamente sin necesidad de refactorizar</t>
   </si>
   <si>
-    <t>a) Deberíamos tener una propiedad en la clase del tipo concreto "EquipoRepository" e inicializarla en el constructor por default</t>
-  </si>
-  <si>
     <t>d) Hacer las inserciones adecuadas en el TestInitialization para poder testear el método</t>
   </si>
   <si>
@@ -171,6 +168,24 @@
   </si>
   <si>
     <t>d) Tiene dependencias de objetos dificiles de instanciar</t>
+  </si>
+  <si>
+    <t>a) Deberíamos tener una propiedad en la clase del tipo concreto "EquipoRepository" e instanciarla en el constructor por default</t>
+  </si>
+  <si>
+    <t>¿Cuál es el objetivo fundamental de utilizar estas prácticas?</t>
+  </si>
+  <si>
+    <t>a) Facturar más horas al cliente</t>
+  </si>
+  <si>
+    <t>b) Mejorar la calidad del producto final</t>
+  </si>
+  <si>
+    <t>d) Vender humo en la Comunidad de Práctica</t>
+  </si>
+  <si>
+    <t>c) Sumar puntos de contribución</t>
   </si>
 </sst>
 </file>
@@ -510,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M57"/>
+  <dimension ref="B1:M63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +606,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -606,158 +621,183 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C42" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D51" s="1"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>